<commit_message>
PLEASE LOOK AT THIS COMMIT: Just updated our task sheet and I'm hoping everyone takes a look so were all on the same page for what were doing this week. Succeed or do not, there is no try and there are no exceptions. Keep your heads up, we have a plan, so lets stick to it...
</commit_message>
<xml_diff>
--- a/Shared Files/TASK_CALENDAR.xlsx
+++ b/Shared Files/TASK_CALENDAR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.painter\Desktop\swole_team_6\Shared Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshx_000\Documents\swole_team_6\Shared Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve"> Week 1</t>
   </si>
@@ -77,18 +77,12 @@
     <t>using the binary map</t>
   </si>
   <si>
-    <t>Finalize tutorial</t>
-  </si>
-  <si>
     <t>Technical Design Guide</t>
   </si>
   <si>
     <t>Design Guide</t>
   </si>
   <si>
-    <t>Start collecting sounds to use, look into FMOD</t>
-  </si>
-  <si>
     <t>Audio Guide</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>Finalize basic editor</t>
   </si>
   <si>
-    <t>Impliment sound system, finalize all event systems</t>
-  </si>
-  <si>
     <t>Custom events, Serialization</t>
   </si>
   <si>
@@ -111,6 +102,24 @@
   </si>
   <si>
     <t xml:space="preserve">Tutorial: finish with 2 to 3 more segments </t>
+  </si>
+  <si>
+    <t>Start collecting sounds to use</t>
+  </si>
+  <si>
+    <t>Finalize tutorial, work on level design</t>
+  </si>
+  <si>
+    <t>finalize all event systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMOD Studio/FMOD sounds </t>
+  </si>
+  <si>
+    <t>Finalize sound system</t>
+  </si>
+  <si>
+    <t>Polish and refine last minute issues</t>
   </si>
 </sst>
 </file>
@@ -431,7 +440,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,30 +475,35 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -497,19 +511,22 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>11</v>
       </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
@@ -529,16 +546,19 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -546,7 +566,7 @@
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wtf is going on...
</commit_message>
<xml_diff>
--- a/Shared Files/TASK_CALENDAR.xlsx
+++ b/Shared Files/TASK_CALENDAR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joshx_000\Documents\swole_team_6\Shared Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.painter\Desktop\swole_team_6\Shared Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve"> Week 1</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Start next level segment (map)</t>
   </si>
   <si>
-    <t>Editor: Scale, Rotate, Edit Values, and Delete</t>
-  </si>
-  <si>
     <t>Window: fullscreen on start, handle CTRL + Alt + DEL</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>Audio Guide</t>
   </si>
   <si>
-    <t>Help with editor and Lua scripts</t>
-  </si>
-  <si>
     <t>Finalize basic editor</t>
   </si>
   <si>
@@ -110,16 +104,19 @@
     <t>Finalize tutorial, work on level design</t>
   </si>
   <si>
-    <t>finalize all event systems</t>
-  </si>
-  <si>
     <t xml:space="preserve">FMOD Studio/FMOD sounds </t>
   </si>
   <si>
-    <t>Finalize sound system</t>
-  </si>
-  <si>
     <t>Polish and refine last minute issues</t>
+  </si>
+  <si>
+    <t>Editor: Camera, Reload, Terxture, Entities</t>
+  </si>
+  <si>
+    <t>finalize collision events and grounded</t>
+  </si>
+  <si>
+    <t>Zilch/JSON</t>
   </si>
 </sst>
 </file>
@@ -440,7 +437,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,35 +472,35 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -511,26 +508,23 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -538,7 +532,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -546,27 +540,27 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
         <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the rubric and scheduling (PLEASE READ)
</commit_message>
<xml_diff>
--- a/Shared Files/TASK_CALENDAR.xlsx
+++ b/Shared Files/TASK_CALENDAR.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve"> Week 1</t>
   </si>
@@ -117,6 +117,42 @@
   </si>
   <si>
     <t>Zilch/JSON</t>
+  </si>
+  <si>
+    <t>Insert sound events for walking and</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> background music on start</t>
+  </si>
+  <si>
+    <t>Finish prototype segment: Level 1</t>
+  </si>
+  <si>
+    <t>Start working in engine</t>
+  </si>
+  <si>
+    <t>Start work in engine</t>
+  </si>
+  <si>
+    <t>find more sound assets</t>
+  </si>
+  <si>
+    <t>make UI assets (at least placeholder?)</t>
+  </si>
+  <si>
+    <t>Cheat Codes: Reload Level shortcut, Load Next Level</t>
+  </si>
+  <si>
+    <t>start Audio Guide</t>
+  </si>
+  <si>
+    <t>Start Art Guide</t>
+  </si>
+  <si>
+    <t>Art Guide</t>
+  </si>
+  <si>
+    <t>Particle Effects</t>
   </si>
 </sst>
 </file>
@@ -437,7 +473,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,32 +543,67 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
       <c r="D6" t="s">
         <v>19</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
       </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
       </c>
+      <c r="F7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
+      <c r="B9" t="s">
+        <v>40</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -556,6 +627,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Better organized Level tools
This is the start of my improvement of the editor that i talked about in slack. I don't think this is buggy, but I didn't check it as thoroughly as i usually check
</commit_message>
<xml_diff>
--- a/Shared Files/TASK_CALENDAR.xlsx
+++ b/Shared Files/TASK_CALENDAR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.painter\Desktop\swole_team_6\Shared Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c.lavelle\Desktop\Repo\Shared Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -92,9 +92,6 @@
     <t xml:space="preserve">Finalize raycasting, finalize </t>
   </si>
   <si>
-    <t>Editor, Reactive</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tutorial: finish with 2 to 3 more segments </t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>Polish and refine last minute issues</t>
   </si>
   <si>
-    <t>Editor: Camera, Reload, Terxture, Entities</t>
-  </si>
-  <si>
     <t>finalize collision events and grounded</t>
   </si>
   <si>
@@ -153,6 +147,12 @@
   </si>
   <si>
     <t>Particle Effects</t>
+  </si>
+  <si>
+    <t>Editor, Reactive. DONE</t>
+  </si>
+  <si>
+    <t>Editor: Camera DONE, Reload DONE, Terxture, Entities</t>
   </si>
 </sst>
 </file>
@@ -508,13 +508,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -544,58 +544,58 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
       </c>
       <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
         <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
         <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -603,7 +603,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -611,7 +611,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
NEW TASK Update and rubric changes
</commit_message>
<xml_diff>
--- a/Shared Files/TASK_CALENDAR.xlsx
+++ b/Shared Files/TASK_CALENDAR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c.lavelle\Desktop\Repo\Shared Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.painter\Desktop\swole_team_6\Shared Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve"> Week 1</t>
   </si>
@@ -146,13 +146,28 @@
     <t>Art Guide</t>
   </si>
   <si>
-    <t>Particle Effects</t>
-  </si>
-  <si>
     <t>Editor, Reactive. DONE</t>
   </si>
   <si>
     <t>Editor: Camera DONE, Reload DONE, Terxture, Entities</t>
+  </si>
+  <si>
+    <t>separate rigidbody and boxcollider</t>
+  </si>
+  <si>
+    <t>finalize tutorial in engine</t>
+  </si>
+  <si>
+    <t>finalize level 1 in engine, menus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCR's: Resolution on start, minimize, fullscreen, </t>
+  </si>
+  <si>
+    <t>editor fixes, work on menus</t>
+  </si>
+  <si>
+    <t>Uninstaller, fix collision event issue, pausing</t>
   </si>
 </sst>
 </file>
@@ -470,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +529,7 @@
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -595,45 +610,64 @@
         <v>38</v>
       </c>
       <c r="D9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>3</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C16" t="s">
         <v>17</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E16" t="s">
         <v>12</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>39</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D17" t="s">
         <v>13</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E17" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
UPDATED TASKS! *PLEASE LOOK*
</commit_message>
<xml_diff>
--- a/Shared Files/TASK_CALENDAR.xlsx
+++ b/Shared Files/TASK_CALENDAR.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t xml:space="preserve"> Week 1</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Week 3</t>
   </si>
   <si>
-    <t>Week 4</t>
-  </si>
-  <si>
     <t>Josh</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>Cheat Codes: god mode, skip to win, skip level</t>
   </si>
   <si>
-    <t>Self-Play</t>
-  </si>
-  <si>
     <t>Uninstall from start menu</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>Design Guide</t>
   </si>
   <si>
-    <t>Audio Guide</t>
-  </si>
-  <si>
     <t>Finalize basic editor</t>
   </si>
   <si>
@@ -152,22 +143,25 @@
     <t>Editor: Camera DONE, Reload DONE, Terxture, Entities</t>
   </si>
   <si>
-    <t>separate rigidbody and boxcollider</t>
-  </si>
-  <si>
-    <t>finalize tutorial in engine</t>
-  </si>
-  <si>
-    <t>finalize level 1 in engine, menus</t>
-  </si>
-  <si>
     <t xml:space="preserve">TCR's: Resolution on start, minimize, fullscreen, </t>
   </si>
   <si>
-    <t>editor fixes, work on menus</t>
-  </si>
-  <si>
-    <t>Uninstaller, fix collision event issue, pausing</t>
+    <t>Implement AI and HUD</t>
+  </si>
+  <si>
+    <t>Implement tutorial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finalize zilch/work on polishing any issues </t>
+  </si>
+  <si>
+    <t>Work on your guide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editor fixes, work on menus, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement an auto play </t>
   </si>
 </sst>
 </file>
@@ -488,7 +482,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,19 +497,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -523,35 +517,35 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -559,116 +553,119 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
         <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>46</v>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>